<commit_message>
Added DK prefix to 0184
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.5.xlsx
+++ b/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD0A06D-E622-4084-9D84-7797FBD11FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44362D4-E728-4B03-AAB3-0EF51458F3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Philip Helger:</t>
         </r>
@@ -45,7 +45,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 ISO6523 identifier</t>
@@ -1532,9 +1532,6 @@
 Check number: mod11 (weights: 5, 4, 3, 2, 7, 6, 5, 4)</t>
   </si>
   <si>
-    <t>RegEx: [0-9]{8}([0-9]{2})?</t>
-  </si>
-  <si>
     <t>RegEx: [0-9]{20}</t>
   </si>
   <si>
@@ -1906,6 +1903,9 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>RegEx: DK[0-9]{8}([0-9]{2})?</t>
   </si>
 </sst>
 </file>
@@ -1944,14 +1944,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2002,7 +2002,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2063,15 +2063,6 @@
     </xf>
     <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2738,10 +2729,10 @@
   <dimension ref="A1:AMN99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2760,7 +2751,7 @@
     <col min="12" max="12" width="30.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30.5703125" style="10" customWidth="1"/>
     <col min="14" max="14" width="24.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" style="24" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" style="10" customWidth="1"/>
     <col min="16" max="1027" width="14.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2781,16 +2772,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>491</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>499</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>500</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>5</v>
@@ -2807,8 +2798,8 @@
       <c r="N1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="23" t="s">
-        <v>537</v>
+      <c r="O1" s="6" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -2831,7 +2822,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>366</v>
@@ -2848,8 +2839,8 @@
       <c r="N2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="24" t="s">
-        <v>538</v>
+      <c r="O2" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -2872,7 +2863,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>367</v>
@@ -2886,8 +2877,8 @@
       <c r="M3" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="O3" s="24" t="s">
-        <v>538</v>
+      <c r="O3" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -2910,7 +2901,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>368</v>
@@ -2924,8 +2915,8 @@
       <c r="M4" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="O4" s="24" t="s">
-        <v>538</v>
+      <c r="O4" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -2948,7 +2939,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>369</v>
@@ -2960,13 +2951,13 @@
         <v>390</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="O5" s="24" t="s">
-        <v>538</v>
+      <c r="O5" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="105" x14ac:dyDescent="0.25">
@@ -2989,7 +2980,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>370</v>
@@ -3006,8 +2997,8 @@
       <c r="N6" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="O6" s="24" t="s">
-        <v>538</v>
+      <c r="O6" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -3030,7 +3021,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>48</v>
@@ -3047,8 +3038,8 @@
       <c r="N7" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="O7" s="24" t="s">
-        <v>538</v>
+      <c r="O7" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="195" x14ac:dyDescent="0.25">
@@ -3071,7 +3062,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>371</v>
@@ -3082,8 +3073,8 @@
       <c r="M8" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="O8" s="24" t="s">
-        <v>538</v>
+      <c r="O8" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="180" x14ac:dyDescent="0.25">
@@ -3106,7 +3097,7 @@
         <v>13</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>372</v>
@@ -3120,8 +3111,8 @@
       <c r="N9" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="O9" s="24" t="s">
-        <v>538</v>
+      <c r="O9" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="210" x14ac:dyDescent="0.25">
@@ -3144,7 +3135,7 @@
         <v>58</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>373</v>
@@ -3158,8 +3149,8 @@
       <c r="N10" s="7" t="s">
         <v>406</v>
       </c>
-      <c r="O10" s="24" t="s">
-        <v>538</v>
+      <c r="O10" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -3182,7 +3173,7 @@
         <v>63</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>64</v>
@@ -3193,8 +3184,8 @@
       <c r="N11" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="O11" s="24" t="s">
-        <v>538</v>
+      <c r="O11" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -3217,7 +3208,7 @@
         <v>13</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>73</v>
@@ -3228,8 +3219,8 @@
       <c r="N12" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="O12" s="24" t="s">
-        <v>538</v>
+      <c r="O12" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -3252,7 +3243,7 @@
         <v>13</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>127</v>
@@ -3263,8 +3254,8 @@
       <c r="N13" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="O13" s="24" t="s">
-        <v>538</v>
+      <c r="O13" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="240" x14ac:dyDescent="0.25">
@@ -3287,7 +3278,7 @@
         <v>79</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>374</v>
@@ -3304,8 +3295,8 @@
       <c r="N14" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="O14" s="24" t="s">
-        <v>538</v>
+      <c r="O14" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -3328,7 +3319,7 @@
         <v>79</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>339</v>
@@ -3342,8 +3333,8 @@
       <c r="N15" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="O15" s="24" t="s">
-        <v>538</v>
+      <c r="O15" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -3366,7 +3357,7 @@
         <v>84</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>375</v>
@@ -3375,42 +3366,42 @@
         <v>383</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="O16" s="24" t="s">
-        <v>538</v>
+        <v>539</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="17" spans="1:15 1028:1028" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="E17" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>501</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>505</v>
-      </c>
-      <c r="E17" s="7" t="s">
+      <c r="G17" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>506</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>507</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="O17" s="24" t="s">
-        <v>538</v>
+      <c r="O17" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="18" spans="1:15 1028:1028" ht="150" x14ac:dyDescent="0.25">
@@ -3433,7 +3424,7 @@
         <v>89</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>376</v>
@@ -3445,13 +3436,13 @@
         <v>394</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="N18" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="O18" s="24" t="s">
-        <v>538</v>
+      <c r="O18" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="19" spans="1:15 1028:1028" ht="225" x14ac:dyDescent="0.25">
@@ -3474,7 +3465,7 @@
         <v>89</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>377</v>
@@ -3486,13 +3477,13 @@
         <v>395</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="N19" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="O19" s="24" t="s">
-        <v>538</v>
+      <c r="O19" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="20" spans="1:15 1028:1028" ht="60" x14ac:dyDescent="0.25">
@@ -3515,7 +3506,7 @@
         <v>89</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>100</v>
@@ -3527,10 +3518,10 @@
         <v>396</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="O20" s="24" t="s">
-        <v>538</v>
+        <v>441</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="21" spans="1:15 1028:1028" ht="45" x14ac:dyDescent="0.25">
@@ -3553,7 +3544,7 @@
         <v>106</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>107</v>
@@ -3562,10 +3553,10 @@
         <v>32</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="O21" s="24" t="s">
-        <v>538</v>
+        <v>442</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="22" spans="1:15 1028:1028" ht="105" x14ac:dyDescent="0.25">
@@ -3588,7 +3579,7 @@
         <v>63</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>378</v>
@@ -3597,13 +3588,13 @@
         <v>385</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="N22" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="O22" s="24" t="s">
-        <v>538</v>
+      <c r="O22" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="23" spans="1:15 1028:1028" ht="105" x14ac:dyDescent="0.25">
@@ -3626,7 +3617,7 @@
         <v>63</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J23" s="9" t="s">
         <v>379</v>
@@ -3635,10 +3626,10 @@
         <v>386</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>445</v>
-      </c>
-      <c r="O23" s="24" t="s">
-        <v>538</v>
+        <v>444</v>
+      </c>
+      <c r="O23" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="24" spans="1:15 1028:1028" ht="45" x14ac:dyDescent="0.25">
@@ -3661,7 +3652,7 @@
         <v>79</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>348</v>
@@ -3670,10 +3661,10 @@
         <v>349</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>446</v>
-      </c>
-      <c r="O24" s="24" t="s">
-        <v>538</v>
+        <v>445</v>
+      </c>
+      <c r="O24" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="25" spans="1:15 1028:1028" ht="409.5" x14ac:dyDescent="0.25">
@@ -3696,7 +3687,7 @@
         <v>79</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>380</v>
@@ -3705,10 +3696,10 @@
         <v>353</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="O25" s="24" t="s">
-        <v>538</v>
+        <v>446</v>
+      </c>
+      <c r="O25" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="26" spans="1:15 1028:1028" ht="90" x14ac:dyDescent="0.25">
@@ -3731,7 +3722,7 @@
         <v>79</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J26" s="9" t="s">
         <v>123</v>
@@ -3743,10 +3734,10 @@
         <v>397</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>448</v>
-      </c>
-      <c r="O26" s="24" t="s">
-        <v>538</v>
+        <v>447</v>
+      </c>
+      <c r="O26" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="27" spans="1:15 1028:1028" ht="30" x14ac:dyDescent="0.25">
@@ -3769,7 +3760,7 @@
         <v>359</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J27" s="9" t="s">
         <v>360</v>
@@ -3779,13 +3770,13 @@
       </c>
       <c r="L27" s="11"/>
       <c r="M27" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="N27" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="O27" s="24" t="s">
-        <v>538</v>
+      <c r="O27" s="10" t="s">
+        <v>537</v>
       </c>
       <c r="AMN27" s="7"/>
     </row>
@@ -3800,7 +3791,7 @@
         <v>226</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>364</v>
@@ -3809,58 +3800,58 @@
         <v>359</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>365</v>
       </c>
       <c r="L28" s="11"/>
       <c r="M28" s="11" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="O28" s="24" t="s">
-        <v>538</v>
+        <v>494</v>
+      </c>
+      <c r="O28" s="10" t="s">
+        <v>537</v>
       </c>
       <c r="AMN28" s="7"/>
     </row>
     <row r="29" spans="1:15 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>532</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>533</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D29" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="J29" s="9" t="s">
         <v>534</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>472</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>535</v>
       </c>
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
       <c r="N29" s="7" t="s">
-        <v>536</v>
-      </c>
-      <c r="O29" s="24" t="s">
-        <v>539</v>
+        <v>535</v>
+      </c>
+      <c r="O29" s="10" t="s">
+        <v>538</v>
       </c>
       <c r="AMN29" s="7"/>
     </row>
@@ -3884,281 +3875,281 @@
         <v>425</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>426</v>
       </c>
       <c r="L30" s="11"/>
       <c r="M30" s="10" t="s">
-        <v>458</v>
-      </c>
-      <c r="O30" s="24" t="s">
-        <v>538</v>
+        <v>457</v>
+      </c>
+      <c r="O30" s="10" t="s">
+        <v>537</v>
       </c>
       <c r="AMN30" s="7"/>
     </row>
     <row r="31" spans="1:15 1028:1028" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>463</v>
-      </c>
-      <c r="F31" s="12" t="s">
+      <c r="G31" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="J31" s="9" t="s">
         <v>465</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>466</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L31" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="M31" s="10" t="s">
-        <v>467</v>
-      </c>
-      <c r="O31" s="24" t="s">
-        <v>538</v>
+        <v>466</v>
+      </c>
+      <c r="O31" s="10" t="s">
+        <v>537</v>
       </c>
       <c r="AMN31" s="7"/>
     </row>
     <row r="32" spans="1:15 1028:1028" ht="255" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D32" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="F32" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="J32" s="9" t="s">
         <v>472</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>465</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>473</v>
       </c>
       <c r="L32" s="11"/>
       <c r="M32" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="O32" s="24" t="s">
-        <v>538</v>
+        <v>473</v>
+      </c>
+      <c r="O32" s="10" t="s">
+        <v>537</v>
       </c>
       <c r="AMN32" s="7"/>
     </row>
     <row r="33" spans="1:1028" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L33" s="11"/>
       <c r="M33" s="10" t="s">
-        <v>452</v>
-      </c>
-      <c r="O33" s="24" t="s">
-        <v>538</v>
+        <v>451</v>
+      </c>
+      <c r="O33" s="10" t="s">
+        <v>537</v>
       </c>
       <c r="AMN33" s="7"/>
     </row>
     <row r="34" spans="1:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>476</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>477</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="F34" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="J34" s="9" t="s">
         <v>481</v>
       </c>
-      <c r="F34" s="12" t="s">
-        <v>465</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="J34" s="9" t="s">
+      <c r="K34" s="9" t="s">
         <v>482</v>
-      </c>
-      <c r="K34" s="9" t="s">
-        <v>483</v>
       </c>
       <c r="L34" s="11"/>
       <c r="M34" s="10" t="s">
-        <v>484</v>
-      </c>
-      <c r="O34" s="24" t="s">
-        <v>538</v>
+        <v>483</v>
+      </c>
+      <c r="O34" s="10" t="s">
+        <v>537</v>
       </c>
       <c r="AMN34" s="7"/>
     </row>
     <row r="35" spans="1:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>478</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>479</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="J35" s="9" t="s">
         <v>485</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>481</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>465</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="J35" s="9" t="s">
+      <c r="K35" s="9" t="s">
         <v>486</v>
-      </c>
-      <c r="K35" s="9" t="s">
-        <v>487</v>
       </c>
       <c r="L35" s="11"/>
       <c r="M35" s="10" t="s">
-        <v>488</v>
-      </c>
-      <c r="O35" s="24" t="s">
-        <v>538</v>
+        <v>487</v>
+      </c>
+      <c r="O35" s="10" t="s">
+        <v>537</v>
       </c>
       <c r="AMN35" s="7"/>
     </row>
     <row r="36" spans="1:1028" ht="150" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>508</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>509</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>510</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="F36" s="12" t="s">
+        <v>501</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="J36" s="9" t="s">
         <v>511</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>502</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>512</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L36" s="11"/>
       <c r="M36" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>513</v>
-      </c>
-      <c r="O36" s="24" t="s">
-        <v>538</v>
+        <v>512</v>
+      </c>
+      <c r="O36" s="10" t="s">
+        <v>537</v>
       </c>
       <c r="AMN36" s="7"/>
     </row>
     <row r="37" spans="1:1028" ht="240" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>515</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>516</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D37" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="E37" s="7" t="s">
         <v>517</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="F37" s="12" t="s">
+        <v>501</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="J37" s="9" t="s">
         <v>518</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>502</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>519</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L37" s="11"/>
       <c r="M37" s="10" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>520</v>
-      </c>
-      <c r="O37" s="24" t="s">
-        <v>538</v>
+        <v>519</v>
+      </c>
+      <c r="O37" s="10" t="s">
+        <v>537</v>
       </c>
       <c r="AMN37" s="7"/>
     </row>
@@ -4182,7 +4173,7 @@
         <v>13</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J38" s="9" t="s">
         <v>127</v>
@@ -4193,8 +4184,8 @@
       <c r="N38" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="O38" s="24" t="s">
-        <v>538</v>
+      <c r="O38" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="39" spans="1:1028" ht="45" x14ac:dyDescent="0.25">
@@ -4217,16 +4208,16 @@
         <v>13</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L39" s="10" t="s">
         <v>398</v>
       </c>
       <c r="M39" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="O39" s="24" t="s">
-        <v>538</v>
+        <v>449</v>
+      </c>
+      <c r="O39" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="40" spans="1:1028" ht="45" x14ac:dyDescent="0.25">
@@ -4249,16 +4240,16 @@
         <v>13</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L40" s="10" t="s">
         <v>134</v>
       </c>
       <c r="M40" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="O40" s="24" t="s">
-        <v>538</v>
+        <v>450</v>
+      </c>
+      <c r="O40" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="41" spans="1:1028" ht="45" x14ac:dyDescent="0.25">
@@ -4281,7 +4272,7 @@
         <v>13</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L41" s="10" t="s">
         <v>134</v>
@@ -4289,8 +4280,8 @@
       <c r="N41" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="O41" s="24" t="s">
-        <v>538</v>
+      <c r="O41" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="42" spans="1:1028" s="20" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -4311,27 +4302,27 @@
         <v>13</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I42" s="18">
         <v>45070</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K42" s="19"/>
       <c r="L42" s="17" t="s">
         <v>141</v>
       </c>
       <c r="M42" s="17" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="N42" s="15"/>
-      <c r="O42" s="25" t="s">
-        <v>539</v>
+      <c r="O42" s="17" t="s">
+        <v>538</v>
       </c>
       <c r="P42" s="15"/>
       <c r="Q42" s="15"/>
@@ -5366,10 +5357,10 @@
         <v>13</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I43" s="18">
         <v>45070</v>
@@ -5380,13 +5371,13 @@
         <v>399</v>
       </c>
       <c r="M43" s="17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="N43" s="15" t="s">
         <v>415</v>
       </c>
-      <c r="O43" s="25" t="s">
-        <v>539</v>
+      <c r="O43" s="17" t="s">
+        <v>538</v>
       </c>
       <c r="P43" s="15"/>
       <c r="Q43" s="15"/>
@@ -6421,10 +6412,10 @@
         <v>13</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I44" s="18">
         <v>45070</v>
@@ -6435,13 +6426,13 @@
       <c r="K44" s="19"/>
       <c r="L44" s="17"/>
       <c r="M44" s="17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="N44" s="15" t="s">
-        <v>529</v>
-      </c>
-      <c r="O44" s="25" t="s">
-        <v>539</v>
+        <v>528</v>
+      </c>
+      <c r="O44" s="17" t="s">
+        <v>538</v>
       </c>
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
@@ -7476,7 +7467,7 @@
         <v>13</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H45" s="8" t="s">
         <v>150</v>
@@ -7485,13 +7476,13 @@
         <v>155</v>
       </c>
       <c r="M45" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="N45" s="7" t="s">
         <v>416</v>
       </c>
-      <c r="O45" s="24" t="s">
-        <v>538</v>
+      <c r="O45" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="46" spans="1:1028" ht="90" x14ac:dyDescent="0.25">
@@ -7511,13 +7502,13 @@
         <v>13</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="M46" s="10" t="s">
-        <v>455</v>
-      </c>
-      <c r="O46" s="24" t="s">
-        <v>538</v>
+        <v>454</v>
+      </c>
+      <c r="O46" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="47" spans="1:1028" ht="75" x14ac:dyDescent="0.25">
@@ -7538,7 +7529,7 @@
         <v>13</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H47" s="8" t="s">
         <v>150</v>
@@ -7547,13 +7538,13 @@
         <v>159</v>
       </c>
       <c r="M47" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="N47" s="7" t="s">
-        <v>459</v>
-      </c>
-      <c r="O47" s="24" t="s">
-        <v>538</v>
+        <v>458</v>
+      </c>
+      <c r="O47" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="48" spans="1:1028" x14ac:dyDescent="0.25">
@@ -7576,13 +7567,13 @@
         <v>13</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="N48" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="O48" s="24" t="s">
-        <v>538</v>
+      <c r="O48" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -7602,13 +7593,13 @@
         <v>13</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L49" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="O49" s="24" t="s">
-        <v>538</v>
+      <c r="O49" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -7629,19 +7620,19 @@
         <v>13</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L50" s="10" t="s">
         <v>400</v>
       </c>
       <c r="M50" s="10" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="N50" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="O50" s="24" t="s">
-        <v>538</v>
+      <c r="O50" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -7661,13 +7652,13 @@
         <v>13</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="O51" s="24" t="s">
-        <v>538</v>
+      <c r="O51" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="105" x14ac:dyDescent="0.25">
@@ -7687,7 +7678,7 @@
         <v>13</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>63</v>
@@ -7699,13 +7690,13 @@
         <v>386</v>
       </c>
       <c r="M52" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="N52" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="O52" s="24" t="s">
-        <v>538</v>
+      <c r="O52" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -7728,13 +7719,13 @@
         <v>183</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J53" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="O53" s="24" t="s">
-        <v>538</v>
+      <c r="O53" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -7755,7 +7746,7 @@
         <v>176</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J54" s="9" t="s">
         <v>187</v>
@@ -7763,8 +7754,8 @@
       <c r="N54" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="O54" s="24" t="s">
-        <v>538</v>
+      <c r="O54" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -7787,10 +7778,10 @@
         <v>176</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O55" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O55" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -7813,7 +7804,7 @@
         <v>150</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H56" s="8" t="s">
         <v>359</v>
@@ -7821,8 +7812,8 @@
       <c r="N56" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="O56" s="24" t="s">
-        <v>538</v>
+      <c r="O56" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -7843,10 +7834,10 @@
         <v>150</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O57" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O57" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -7867,10 +7858,10 @@
         <v>150</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O58" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O58" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -7891,10 +7882,10 @@
         <v>150</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O59" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O59" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -7915,10 +7906,10 @@
         <v>150</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O60" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O60" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -7939,10 +7930,10 @@
         <v>150</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O61" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O61" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -7963,10 +7954,10 @@
         <v>150</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O62" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O62" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -7986,10 +7977,10 @@
         <v>150</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O63" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O63" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
@@ -8010,10 +8001,10 @@
         <v>150</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O64" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O64" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
@@ -8034,10 +8025,10 @@
         <v>150</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O65" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O65" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
@@ -8058,10 +8049,10 @@
         <v>150</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O66" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O66" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
@@ -8082,10 +8073,10 @@
         <v>150</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O67" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O67" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
@@ -8106,10 +8097,10 @@
         <v>150</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O68" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O68" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
@@ -8130,10 +8121,10 @@
         <v>150</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O69" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O69" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
@@ -8154,10 +8145,10 @@
         <v>150</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O70" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O70" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
@@ -8178,10 +8169,10 @@
         <v>150</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O71" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O71" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
@@ -8202,10 +8193,10 @@
         <v>150</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O72" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O72" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
@@ -8226,10 +8217,10 @@
         <v>150</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O73" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O73" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
@@ -8250,10 +8241,10 @@
         <v>150</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O74" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O74" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
@@ -8274,10 +8265,10 @@
         <v>150</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O75" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O75" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
@@ -8298,10 +8289,10 @@
         <v>150</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O76" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O76" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -8322,10 +8313,10 @@
         <v>150</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O77" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O77" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
@@ -8346,10 +8337,10 @@
         <v>150</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O78" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O78" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
@@ -8370,10 +8361,10 @@
         <v>150</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O79" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O79" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
@@ -8394,10 +8385,10 @@
         <v>150</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O80" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O80" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="81" spans="1:1027" x14ac:dyDescent="0.25">
@@ -8418,10 +8409,10 @@
         <v>150</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O81" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O81" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="82" spans="1:1027" x14ac:dyDescent="0.25">
@@ -8442,11 +8433,11 @@
         <v>150</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I82" s="3"/>
-      <c r="O82" s="24" t="s">
-        <v>538</v>
+      <c r="O82" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="83" spans="1:1027" x14ac:dyDescent="0.25">
@@ -8467,11 +8458,11 @@
         <v>150</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I83" s="3"/>
-      <c r="O83" s="24" t="s">
-        <v>538</v>
+      <c r="O83" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="84" spans="1:1027" x14ac:dyDescent="0.25">
@@ -8492,11 +8483,11 @@
         <v>150</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I84" s="3"/>
-      <c r="O84" s="24" t="s">
-        <v>538</v>
+      <c r="O84" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="85" spans="1:1027" x14ac:dyDescent="0.25">
@@ -8517,10 +8508,10 @@
         <v>150</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O85" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O85" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="86" spans="1:1027" x14ac:dyDescent="0.25">
@@ -8540,10 +8531,10 @@
         <v>150</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O86" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O86" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="87" spans="1:1027" x14ac:dyDescent="0.25">
@@ -8564,11 +8555,11 @@
         <v>150</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I87" s="4"/>
-      <c r="O87" s="24" t="s">
-        <v>538</v>
+      <c r="O87" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="88" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
@@ -8589,10 +8580,10 @@
         <v>150</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O88" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O88" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="89" spans="1:1027" x14ac:dyDescent="0.25">
@@ -8612,7 +8603,7 @@
         <v>320</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H89" s="8" t="s">
         <v>89</v>
@@ -8621,8 +8612,8 @@
       <c r="N89" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="O89" s="24" t="s">
-        <v>538</v>
+      <c r="O89" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="90" spans="1:1027" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -8643,10 +8634,10 @@
         <v>325</v>
       </c>
       <c r="G90" s="17" t="s">
+        <v>529</v>
+      </c>
+      <c r="H90" s="16" t="s">
         <v>530</v>
-      </c>
-      <c r="H90" s="16" t="s">
-        <v>531</v>
       </c>
       <c r="I90" s="22">
         <v>45138</v>
@@ -8656,8 +8647,8 @@
       <c r="L90" s="17"/>
       <c r="M90" s="17"/>
       <c r="N90" s="15"/>
-      <c r="O90" s="25" t="s">
-        <v>539</v>
+      <c r="O90" s="17" t="s">
+        <v>538</v>
       </c>
       <c r="P90" s="15"/>
       <c r="Q90" s="15"/>
@@ -9692,10 +9683,10 @@
         <v>84</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I91" s="3"/>
       <c r="J91" s="9" t="s">
@@ -9705,10 +9696,10 @@
         <v>401</v>
       </c>
       <c r="M91" s="10" t="s">
-        <v>458</v>
-      </c>
-      <c r="O91" s="24" t="s">
-        <v>538</v>
+        <v>457</v>
+      </c>
+      <c r="O91" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="92" spans="1:1027" x14ac:dyDescent="0.25">
@@ -9728,10 +9719,10 @@
         <v>84</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O92" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O92" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="93" spans="1:1027" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -9745,14 +9736,14 @@
         <v>226</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E93" s="15"/>
       <c r="F93" s="16" t="s">
         <v>106</v>
       </c>
       <c r="G93" s="17" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H93" s="16" t="s">
         <v>359</v>
@@ -9767,8 +9758,8 @@
       <c r="N93" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="O93" s="25" t="s">
-        <v>539</v>
+      <c r="O93" s="17" t="s">
+        <v>538</v>
       </c>
       <c r="P93" s="15"/>
       <c r="Q93" s="15"/>
@@ -10785,25 +10776,25 @@
     </row>
     <row r="94" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="B94" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="C94" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="C94" s="7" t="s">
+      <c r="D94" s="7" t="s">
         <v>524</v>
       </c>
-      <c r="D94" s="7" t="s">
-        <v>525</v>
-      </c>
       <c r="F94" s="8" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="O94" s="24" t="s">
-        <v>538</v>
+        <v>491</v>
+      </c>
+      <c r="O94" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="99" spans="9:9" x14ac:dyDescent="0.25">

</xml_diff>